<commit_message>
Do full hour for 1 grade
</commit_message>
<xml_diff>
--- a/Zaizd2.xlsx
+++ b/Zaizd2.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\rozklad\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="300" windowWidth="20730" windowHeight="9480"/>
   </bookViews>
@@ -16,9 +21,9 @@
     <sheet name="7 курс" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'1 курс'!$A$1:$M$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'1 курс'!$A$1:$N$15</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -28,7 +33,7 @@
     <author>xgresx@gmail.com</author>
   </authors>
   <commentList>
-    <comment ref="I15" authorId="0">
+    <comment ref="J15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +58,7 @@
     <author>user</author>
   </authors>
   <commentList>
-    <comment ref="B24" authorId="0">
+    <comment ref="B24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +83,7 @@
     <author>xgresx@gmail.com</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0">
+    <comment ref="I9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +124,7 @@
     <author>user</author>
   </authors>
   <commentList>
-    <comment ref="I25" authorId="0">
+    <comment ref="I25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -135,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B40" authorId="1">
+    <comment ref="B40" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -161,7 +166,7 @@
     <author>xgresx@gmail.com</author>
   </authors>
   <commentList>
-    <comment ref="B10" authorId="0">
+    <comment ref="B10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0">
+    <comment ref="B14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -191,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0">
+    <comment ref="B15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -217,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="1">
+    <comment ref="I18" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -242,7 +247,7 @@
     <author>user</author>
   </authors>
   <commentList>
-    <comment ref="B18" authorId="0">
+    <comment ref="B18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -257,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B34" authorId="0">
+    <comment ref="B34" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -277,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="316">
   <si>
     <t>Групи</t>
   </si>
@@ -1222,12 +1227,15 @@
   </si>
   <si>
     <t>Годин 4 заїзд</t>
+  </si>
+  <si>
+    <t>Використано годин</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1817,11 +1825,11 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Ввід" xfId="3" builtinId="20"/>
-    <cellStyle name="Добре" xfId="1" builtinId="26"/>
+    <cellStyle name="Гарний" xfId="1" builtinId="26"/>
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
-    <cellStyle name="Середній" xfId="2" builtinId="28"/>
+    <cellStyle name="Нейтральний" xfId="2" builtinId="28"/>
   </cellStyles>
-  <dxfs count="98">
+  <dxfs count="99">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1845,340 +1853,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3524,6 +3198,365 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -3543,54 +3576,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:M27" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="15">
-  <autoFilter ref="A1:M27"/>
-  <tableColumns count="13">
-    <tableColumn id="1" name="Групи" dataDxfId="14"/>
-    <tableColumn id="2" name="Дисципліна" dataDxfId="13"/>
-    <tableColumn id="3" name="Годин 1 заїзд" dataDxfId="2"/>
-    <tableColumn id="6" name="Годин 2 заїзд" dataDxfId="12"/>
-    <tableColumn id="14" name="Годин 3 заїзд" dataDxfId="0"/>
-    <tableColumn id="5" name="Годин 4 заїзд" dataDxfId="1"/>
-    <tableColumn id="7" name="Прим." dataDxfId="11"/>
-    <tableColumn id="8" name="шифр спеціальності" dataDxfId="10"/>
-    <tableColumn id="9" name="Викладач" dataDxfId="9"/>
-    <tableColumn id="10" name="Лекц.2" dataDxfId="8"/>
-    <tableColumn id="11" name="Практ.3" dataDxfId="7"/>
-    <tableColumn id="12" name="Лаб." dataDxfId="6"/>
-    <tableColumn id="13" name="Шифр кафедри" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:N27" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
+  <autoFilter ref="A1:N27"/>
+  <tableColumns count="14">
+    <tableColumn id="1" name="Групи" dataDxfId="93"/>
+    <tableColumn id="2" name="Дисципліна" dataDxfId="92"/>
+    <tableColumn id="3" name="Годин 1 заїзд" dataDxfId="91"/>
+    <tableColumn id="6" name="Годин 2 заїзд" dataDxfId="90"/>
+    <tableColumn id="14" name="Годин 3 заїзд" dataDxfId="89"/>
+    <tableColumn id="5" name="Годин 4 заїзд" dataDxfId="88"/>
+    <tableColumn id="15" name="Використано годин" dataDxfId="0"/>
+    <tableColumn id="7" name="Прим." dataDxfId="87"/>
+    <tableColumn id="8" name="шифр спеціальності" dataDxfId="86"/>
+    <tableColumn id="9" name="Викладач" dataDxfId="85"/>
+    <tableColumn id="10" name="Лекц.2" dataDxfId="84"/>
+    <tableColumn id="11" name="Практ.3" dataDxfId="83"/>
+    <tableColumn id="12" name="Лаб." dataDxfId="82"/>
+    <tableColumn id="13" name="Шифр кафедри" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="A1:M31" totalsRowShown="0" headerRowDxfId="97" dataDxfId="95" headerRowBorderDxfId="96" tableBorderDxfId="94" totalsRowBorderDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="A1:M31" totalsRowShown="0" headerRowDxfId="80" dataDxfId="78" headerRowBorderDxfId="79" tableBorderDxfId="77" totalsRowBorderDxfId="76">
   <autoFilter ref="A1:M31"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Групи" dataDxfId="92"/>
-    <tableColumn id="2" name="Дисципліна" dataDxfId="91"/>
-    <tableColumn id="3" name="Лекц." dataDxfId="90"/>
-    <tableColumn id="4" name="Практ." dataDxfId="89"/>
-    <tableColumn id="5" name="Лабор." dataDxfId="88"/>
-    <tableColumn id="6" name="В т. ч.  годин" dataDxfId="87"/>
-    <tableColumn id="7" name="Прим." dataDxfId="86"/>
-    <tableColumn id="8" name="шифр спеціальності" dataDxfId="85"/>
-    <tableColumn id="9" name="Викладач" dataDxfId="84"/>
-    <tableColumn id="10" name="Лекц.2" dataDxfId="83"/>
-    <tableColumn id="11" name="Практ.3" dataDxfId="82"/>
-    <tableColumn id="12" name="Лаб." dataDxfId="81"/>
-    <tableColumn id="13" name="Столбец4" dataDxfId="80"/>
+    <tableColumn id="1" name="Групи" dataDxfId="75"/>
+    <tableColumn id="2" name="Дисципліна" dataDxfId="74"/>
+    <tableColumn id="3" name="Лекц." dataDxfId="73"/>
+    <tableColumn id="4" name="Практ." dataDxfId="72"/>
+    <tableColumn id="5" name="Лабор." dataDxfId="71"/>
+    <tableColumn id="6" name="В т. ч.  годин" dataDxfId="70"/>
+    <tableColumn id="7" name="Прим." dataDxfId="69"/>
+    <tableColumn id="8" name="шифр спеціальності" dataDxfId="68"/>
+    <tableColumn id="9" name="Викладач" dataDxfId="67"/>
+    <tableColumn id="10" name="Лекц.2" dataDxfId="66"/>
+    <tableColumn id="11" name="Практ.3" dataDxfId="65"/>
+    <tableColumn id="12" name="Лаб." dataDxfId="64"/>
+    <tableColumn id="13" name="Столбец4" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Таблица3" displayName="Таблица3" ref="A1:L44" totalsRowShown="0" headerRowDxfId="79" headerRowBorderDxfId="78" tableBorderDxfId="77" totalsRowBorderDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Таблица3" displayName="Таблица3" ref="A1:L44" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60" totalsRowBorderDxfId="59">
   <autoFilter ref="A1:L44"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Групи" dataDxfId="75"/>
+    <tableColumn id="1" name="Групи" dataDxfId="58"/>
     <tableColumn id="2" name="Дисципліна"/>
     <tableColumn id="3" name="Лекц."/>
     <tableColumn id="4" name="Практ."/>
@@ -3601,69 +3635,69 @@
     <tableColumn id="9" name="Викладач"/>
     <tableColumn id="10" name="Лекц.2"/>
     <tableColumn id="11" name="Практ.3"/>
-    <tableColumn id="12" name="Лаб." dataDxfId="74"/>
+    <tableColumn id="12" name="Лаб." dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Таблица4" displayName="Таблица4" ref="A1:L42" totalsRowShown="0" headerRowDxfId="73" headerRowBorderDxfId="72" tableBorderDxfId="71" totalsRowBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Таблица4" displayName="Таблица4" ref="A1:L42" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54" totalsRowBorderDxfId="53">
   <autoFilter ref="A1:L42"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Групи" dataDxfId="69"/>
-    <tableColumn id="2" name="Дисципліна" dataDxfId="68"/>
-    <tableColumn id="3" name="Лекц." dataDxfId="67"/>
-    <tableColumn id="4" name="Практ." dataDxfId="66"/>
-    <tableColumn id="5" name="Лабор." dataDxfId="65"/>
-    <tableColumn id="6" name="В т. ч.  годин" dataDxfId="64"/>
-    <tableColumn id="7" name="Прим." dataDxfId="63"/>
-    <tableColumn id="8" name="Шифр спеціальності" dataDxfId="62"/>
+    <tableColumn id="1" name="Групи" dataDxfId="52"/>
+    <tableColumn id="2" name="Дисципліна" dataDxfId="51"/>
+    <tableColumn id="3" name="Лекц." dataDxfId="50"/>
+    <tableColumn id="4" name="Практ." dataDxfId="49"/>
+    <tableColumn id="5" name="Лабор." dataDxfId="48"/>
+    <tableColumn id="6" name="В т. ч.  годин" dataDxfId="47"/>
+    <tableColumn id="7" name="Прим." dataDxfId="46"/>
+    <tableColumn id="8" name="Шифр спеціальності" dataDxfId="45"/>
     <tableColumn id="9" name="Викладач"/>
     <tableColumn id="10" name="Лекц.2"/>
     <tableColumn id="11" name="Практ.3"/>
-    <tableColumn id="12" name="Лаб." dataDxfId="61"/>
+    <tableColumn id="12" name="Лаб." dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Таблица5" displayName="Таблица5" ref="A1:L27" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="59" tableBorderDxfId="58" totalsRowBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Таблица5" displayName="Таблица5" ref="A1:L27" totalsRowShown="0" headerRowDxfId="43" headerRowBorderDxfId="42" tableBorderDxfId="41" totalsRowBorderDxfId="40">
   <autoFilter ref="A1:L27"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Групи" dataDxfId="56"/>
-    <tableColumn id="2" name="Дисципліна" dataDxfId="55"/>
-    <tableColumn id="3" name="Лекц." dataDxfId="54"/>
-    <tableColumn id="4" name="Практ." dataDxfId="53"/>
-    <tableColumn id="5" name="Лабор." dataDxfId="52"/>
-    <tableColumn id="6" name="В т. ч.  годин" dataDxfId="51"/>
-    <tableColumn id="7" name="Прим." dataDxfId="50"/>
-    <tableColumn id="8" name="Шифр спецільності" dataDxfId="49"/>
-    <tableColumn id="9" name="Викладач" dataDxfId="48"/>
-    <tableColumn id="10" name="Лекц.2" dataDxfId="47"/>
+    <tableColumn id="1" name="Групи" dataDxfId="39"/>
+    <tableColumn id="2" name="Дисципліна" dataDxfId="38"/>
+    <tableColumn id="3" name="Лекц." dataDxfId="37"/>
+    <tableColumn id="4" name="Практ." dataDxfId="36"/>
+    <tableColumn id="5" name="Лабор." dataDxfId="35"/>
+    <tableColumn id="6" name="В т. ч.  годин" dataDxfId="34"/>
+    <tableColumn id="7" name="Прим." dataDxfId="33"/>
+    <tableColumn id="8" name="Шифр спецільності" dataDxfId="32"/>
+    <tableColumn id="9" name="Викладач" dataDxfId="31"/>
+    <tableColumn id="10" name="Лекц.2" dataDxfId="30"/>
     <tableColumn id="11" name="Практ.3"/>
-    <tableColumn id="12" name="Лаб." dataDxfId="46"/>
+    <tableColumn id="12" name="Лаб." dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Таблица6" displayName="Таблица6" ref="A1:L34" totalsRowShown="0" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Таблица6" displayName="Таблица6" ref="A1:L34" totalsRowShown="0" tableBorderDxfId="28">
   <autoFilter ref="A1:L34"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Групи" dataDxfId="44"/>
-    <tableColumn id="2" name="Дисципліна" dataDxfId="43"/>
-    <tableColumn id="3" name="Лекц." dataDxfId="42"/>
-    <tableColumn id="4" name="Практ." dataDxfId="41"/>
-    <tableColumn id="5" name="Лабор." dataDxfId="40"/>
-    <tableColumn id="6" name="В т. ч.  годин" dataDxfId="39"/>
-    <tableColumn id="7" name="Прим." dataDxfId="38"/>
-    <tableColumn id="8" name="Шифр. Спеціальності" dataDxfId="37"/>
-    <tableColumn id="9" name="Викладач" dataDxfId="36"/>
+    <tableColumn id="1" name="Групи" dataDxfId="27"/>
+    <tableColumn id="2" name="Дисципліна" dataDxfId="26"/>
+    <tableColumn id="3" name="Лекц." dataDxfId="25"/>
+    <tableColumn id="4" name="Практ." dataDxfId="24"/>
+    <tableColumn id="5" name="Лабор." dataDxfId="23"/>
+    <tableColumn id="6" name="В т. ч.  годин" dataDxfId="22"/>
+    <tableColumn id="7" name="Прим." dataDxfId="21"/>
+    <tableColumn id="8" name="Шифр. Спеціальності" dataDxfId="20"/>
+    <tableColumn id="9" name="Викладач" dataDxfId="19"/>
     <tableColumn id="10" name="Лекц.2"/>
-    <tableColumn id="11" name="Практ.3" dataDxfId="35"/>
+    <tableColumn id="11" name="Практ.3" dataDxfId="18"/>
     <tableColumn id="12" name="Лаб."/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3671,21 +3705,21 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Таблица7" displayName="Таблица7" ref="A1:L4" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Таблица7" displayName="Таблица7" ref="A1:L4" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:L4"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Групи" dataDxfId="29"/>
-    <tableColumn id="2" name="Дисципліна" dataDxfId="28"/>
-    <tableColumn id="3" name="Лекц." dataDxfId="27"/>
-    <tableColumn id="4" name="Практ." dataDxfId="26"/>
-    <tableColumn id="5" name="Лабор." dataDxfId="25"/>
-    <tableColumn id="6" name="В т. ч.  годин" dataDxfId="24"/>
-    <tableColumn id="7" name="Прим." dataDxfId="23"/>
-    <tableColumn id="8" name="Шифр спецільності" dataDxfId="22"/>
-    <tableColumn id="9" name="Викладач" dataDxfId="21"/>
-    <tableColumn id="10" name="Лекц.2" dataDxfId="20"/>
-    <tableColumn id="11" name="Практ.3" dataDxfId="19"/>
-    <tableColumn id="12" name="Лаб." dataDxfId="18"/>
+    <tableColumn id="1" name="Групи" dataDxfId="12"/>
+    <tableColumn id="2" name="Дисципліна" dataDxfId="11"/>
+    <tableColumn id="3" name="Лекц." dataDxfId="10"/>
+    <tableColumn id="4" name="Практ." dataDxfId="9"/>
+    <tableColumn id="5" name="Лабор." dataDxfId="8"/>
+    <tableColumn id="6" name="В т. ч.  годин" dataDxfId="7"/>
+    <tableColumn id="7" name="Прим." dataDxfId="6"/>
+    <tableColumn id="8" name="Шифр спецільності" dataDxfId="5"/>
+    <tableColumn id="9" name="Викладач" dataDxfId="4"/>
+    <tableColumn id="10" name="Лекц.2" dataDxfId="3"/>
+    <tableColumn id="11" name="Практ.3" dataDxfId="2"/>
+    <tableColumn id="12" name="Лаб." dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3694,7 +3728,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Стандартна">
+    <a:clrScheme name="Офіс">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3732,9 +3766,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартна">
+    <a:fontScheme name="Офіс">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3769,7 +3803,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3804,7 +3838,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартна">
+    <a:fmtScheme name="Офіс">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3978,10 +4012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M238"/>
+  <dimension ref="A1:N238"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3989,18 +4023,18 @@
     <col min="1" max="1" width="19.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="42.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="15.140625" style="3" customWidth="1"/>
-    <col min="4" max="6" width="14.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13" style="3" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="10" style="3" customWidth="1"/>
-    <col min="12" max="12" width="7.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="3"/>
+    <col min="4" max="7" width="14.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="13" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="10" style="3" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="103" t="s">
         <v>0</v>
       </c>
@@ -4020,49 +4054,61 @@
         <v>314</v>
       </c>
       <c r="G1" s="104" t="s">
+        <v>315</v>
+      </c>
+      <c r="H1" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="104" t="s">
+      <c r="I1" s="104" t="s">
         <v>198</v>
       </c>
-      <c r="I1" s="104" t="s">
+      <c r="J1" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="105" t="s">
+      <c r="K1" s="105" t="s">
         <v>274</v>
       </c>
-      <c r="K1" s="105" t="s">
+      <c r="L1" s="105" t="s">
         <v>275</v>
       </c>
-      <c r="L1" s="105" t="s">
+      <c r="M1" s="105" t="s">
         <v>218</v>
       </c>
-      <c r="M1" s="106" t="s">
+      <c r="N1" s="106" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="95" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
+      <c r="C2" s="96">
+        <v>4</v>
+      </c>
+      <c r="D2" s="96">
+        <v>4</v>
+      </c>
+      <c r="E2" s="96">
+        <v>2</v>
+      </c>
       <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="96" t="s">
+      <c r="G2" s="96">
+        <v>0</v>
+      </c>
+      <c r="H2" s="96"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="96" t="s">
         <v>194</v>
       </c>
-      <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
-      <c r="M2" s="42"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M2" s="6"/>
+      <c r="N2" s="42"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="95" t="s">
         <v>8</v>
       </c>
@@ -4075,19 +4121,22 @@
       <c r="D3" s="96">
         <v>6</v>
       </c>
-      <c r="E3" s="96"/>
+      <c r="E3" s="96">
+        <v>4</v>
+      </c>
       <c r="F3" s="96"/>
       <c r="G3" s="96"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="96" t="s">
+      <c r="H3" s="96"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="96" t="s">
         <v>197</v>
       </c>
-      <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
-      <c r="M3" s="42"/>
-    </row>
-    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="M3" s="6"/>
+      <c r="N3" s="42"/>
+    </row>
+    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="95" t="s">
         <v>8</v>
       </c>
@@ -4100,21 +4149,26 @@
       <c r="D4" s="96">
         <v>6</v>
       </c>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96" t="s">
+      <c r="E4" s="96">
+        <v>4</v>
+      </c>
+      <c r="F4" s="96">
+        <v>4</v>
+      </c>
+      <c r="G4" s="96"/>
+      <c r="H4" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="97"/>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="97"/>
+      <c r="J4" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
-      <c r="M4" s="42"/>
-    </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="M4" s="6"/>
+      <c r="N4" s="42"/>
+    </row>
+    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>11</v>
       </c>
@@ -4130,18 +4184,19 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="8"/>
+      <c r="I5" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="J5" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-      <c r="M5" s="42"/>
-    </row>
-    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="M5" s="6"/>
+      <c r="N5" s="42"/>
+    </row>
+    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>11</v>
       </c>
@@ -4156,25 +4211,26 @@
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="8"/>
+      <c r="H6" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="J6" s="6">
+      <c r="K6" s="6">
         <v>12</v>
       </c>
-      <c r="K6" s="6">
-        <v>8</v>
-      </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="42"/>
-    </row>
-    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="L6" s="6">
+        <v>8</v>
+      </c>
+      <c r="M6" s="6"/>
+      <c r="N6" s="42"/>
+    </row>
+    <row r="7" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>11</v>
       </c>
@@ -4189,25 +4245,26 @@
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="8"/>
+      <c r="H7" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="I7" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="J7" s="6">
+      <c r="K7" s="6">
         <v>12</v>
       </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6">
-        <v>8</v>
-      </c>
-      <c r="M7" s="42"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L7" s="6"/>
+      <c r="M7" s="6">
+        <v>8</v>
+      </c>
+      <c r="N7" s="42"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
         <v>11</v>
       </c>
@@ -4223,16 +4280,17 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="8"/>
+      <c r="I8" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="42"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M8" s="6"/>
+      <c r="N8" s="42"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>11</v>
       </c>
@@ -4245,54 +4303,58 @@
       <c r="D9" s="8">
         <v>10</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="8">
+        <v>2</v>
+      </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="8"/>
+      <c r="I9" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="J9" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="J9" s="6">
-        <v>8</v>
-      </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6">
-        <v>6</v>
-      </c>
-      <c r="M9" s="42"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K9" s="6">
+        <v>8</v>
+      </c>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6">
+        <v>6</v>
+      </c>
+      <c r="N9" s="42"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="8">
-        <v>0</v>
-      </c>
+      <c r="C10" s="8"/>
       <c r="D10" s="8">
         <v>4</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8">
+        <v>6</v>
+      </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="8"/>
+      <c r="I10" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="I10" s="26" t="s">
+      <c r="J10" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="J10" s="26">
-        <v>4</v>
-      </c>
-      <c r="K10" s="98"/>
+      <c r="K10" s="26">
+        <v>4</v>
+      </c>
       <c r="L10" s="98"/>
-      <c r="M10" s="42"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M10" s="98"/>
+      <c r="N10" s="42"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
         <v>11</v>
       </c>
@@ -4305,21 +4367,26 @@
       <c r="D11" s="8">
         <v>0</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="E11" s="8">
+        <v>8</v>
+      </c>
+      <c r="F11" s="8">
+        <v>12</v>
+      </c>
       <c r="G11" s="8"/>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="8"/>
+      <c r="I11" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="J11" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
-      <c r="M11" s="42"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M11" s="6"/>
+      <c r="N11" s="42"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
         <v>21</v>
       </c>
@@ -4332,23 +4399,28 @@
       <c r="D12" s="8">
         <v>8</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="E12" s="8">
+        <v>6</v>
+      </c>
+      <c r="F12" s="8">
+        <v>6</v>
+      </c>
       <c r="G12" s="8"/>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="8"/>
+      <c r="I12" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="J12" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
-      <c r="M12" s="42" t="s">
+      <c r="M12" s="6"/>
+      <c r="N12" s="42" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
         <v>195</v>
       </c>
@@ -4361,23 +4433,28 @@
       <c r="D13" s="8">
         <v>8</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="E13" s="8">
+        <v>6</v>
+      </c>
+      <c r="F13" s="8">
+        <v>6</v>
+      </c>
       <c r="G13" s="8"/>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="8"/>
+      <c r="I13" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
-      <c r="M13" s="42" t="s">
+      <c r="M13" s="6"/>
+      <c r="N13" s="42" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
         <v>23</v>
       </c>
@@ -4390,25 +4467,30 @@
       <c r="D14" s="8">
         <v>8</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="E14" s="8">
+        <v>6</v>
+      </c>
+      <c r="F14" s="8">
+        <v>6</v>
+      </c>
       <c r="G14" s="8"/>
-      <c r="H14" s="6">
+      <c r="H14" s="8"/>
+      <c r="I14" s="6">
         <v>6.1929999999999996</v>
       </c>
-      <c r="I14" s="98" t="s">
+      <c r="J14" s="98" t="s">
         <v>213</v>
       </c>
-      <c r="J14" s="98">
-        <v>4</v>
-      </c>
       <c r="K14" s="98">
+        <v>4</v>
+      </c>
+      <c r="L14" s="98">
         <v>0</v>
       </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="42"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M14" s="6"/>
+      <c r="N14" s="42"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
         <v>23</v>
       </c>
@@ -4421,23 +4503,28 @@
       <c r="D15" s="8">
         <v>4</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="E15" s="8">
+        <v>12</v>
+      </c>
+      <c r="F15" s="8">
+        <v>8</v>
+      </c>
       <c r="G15" s="8"/>
-      <c r="H15" s="6">
+      <c r="H15" s="8"/>
+      <c r="I15" s="6">
         <v>6.1929999999999996</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="J15" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="J15" s="6">
+      <c r="K15" s="6">
         <v>2</v>
       </c>
-      <c r="K15" s="6"/>
       <c r="L15" s="6"/>
-      <c r="M15" s="42"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M15" s="6"/>
+      <c r="N15" s="42"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
         <v>23</v>
       </c>
@@ -4450,25 +4537,30 @@
       <c r="D16" s="8">
         <v>8</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+      <c r="E16" s="8">
+        <v>4</v>
+      </c>
+      <c r="F16" s="8">
+        <v>12</v>
+      </c>
       <c r="G16" s="8"/>
-      <c r="H16" s="6">
+      <c r="H16" s="8"/>
+      <c r="I16" s="6">
         <v>6.1929999999999996</v>
       </c>
-      <c r="I16" s="98" t="s">
+      <c r="J16" s="98" t="s">
         <v>211</v>
       </c>
-      <c r="J16" s="98">
-        <v>4</v>
-      </c>
-      <c r="K16" s="98"/>
-      <c r="L16" s="98">
+      <c r="K16" s="98">
+        <v>4</v>
+      </c>
+      <c r="L16" s="98"/>
+      <c r="M16" s="98">
         <v>2</v>
       </c>
-      <c r="M16" s="42"/>
-    </row>
-    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N16" s="42"/>
+    </row>
+    <row r="17" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
         <v>23</v>
       </c>
@@ -4481,87 +4573,96 @@
       <c r="D17" s="8">
         <v>4</v>
       </c>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8">
+        <v>4</v>
+      </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
-      <c r="H17" s="6">
+      <c r="H17" s="8"/>
+      <c r="I17" s="6">
         <v>6.1929999999999996</v>
       </c>
-      <c r="I17" s="98" t="s">
+      <c r="J17" s="98" t="s">
         <v>213</v>
       </c>
-      <c r="J17" s="98">
+      <c r="K17" s="98">
         <v>2</v>
-      </c>
-      <c r="K17" s="98">
-        <v>0</v>
       </c>
       <c r="L17" s="98">
         <v>0</v>
       </c>
-      <c r="M17" s="42"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M17" s="98">
+        <v>0</v>
+      </c>
+      <c r="N17" s="42"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="8"/>
+      <c r="D18" s="8">
+        <v>6</v>
+      </c>
+      <c r="E18" s="8">
+        <v>6</v>
+      </c>
+      <c r="F18" s="8">
+        <v>6</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="6">
+        <v>6.1929999999999996</v>
+      </c>
+      <c r="J18" s="98" t="s">
+        <v>245</v>
+      </c>
+      <c r="K18" s="98">
+        <v>2</v>
+      </c>
+      <c r="L18" s="98"/>
+      <c r="M18" s="98">
         <v>0</v>
       </c>
-      <c r="D18" s="8">
-        <v>6</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="6">
-        <v>6.1929999999999996</v>
-      </c>
-      <c r="I18" s="98" t="s">
-        <v>245</v>
-      </c>
-      <c r="J18" s="98">
-        <v>2</v>
-      </c>
-      <c r="K18" s="98"/>
-      <c r="L18" s="98">
-        <v>0</v>
-      </c>
-      <c r="M18" s="42"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="42"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="8">
-        <v>0</v>
-      </c>
+      <c r="C19" s="8"/>
       <c r="D19" s="8">
         <v>4</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="E19" s="8">
+        <v>4</v>
+      </c>
+      <c r="F19" s="8">
+        <v>4</v>
+      </c>
       <c r="G19" s="8"/>
-      <c r="H19" s="6">
+      <c r="H19" s="8"/>
+      <c r="I19" s="6">
         <v>6.1929999999999996</v>
       </c>
-      <c r="I19" s="98" t="s">
+      <c r="J19" s="98" t="s">
         <v>210</v>
       </c>
-      <c r="J19" s="98">
+      <c r="K19" s="98">
         <v>2</v>
       </c>
-      <c r="K19" s="98"/>
       <c r="L19" s="98"/>
-      <c r="M19" s="42"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M19" s="98"/>
+      <c r="N19" s="42"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
         <v>30</v>
       </c>
@@ -4580,23 +4681,24 @@
       <c r="F20" s="6">
         <v>8</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="6">
+      <c r="G20" s="6"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="6">
         <v>6.2050000000000001</v>
       </c>
-      <c r="I20" s="98" t="s">
+      <c r="J20" s="98" t="s">
         <v>214</v>
       </c>
-      <c r="J20" s="98">
-        <v>6</v>
-      </c>
-      <c r="K20" s="98"/>
-      <c r="L20" s="98">
-        <v>4</v>
-      </c>
-      <c r="M20" s="42"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K20" s="98">
+        <v>6</v>
+      </c>
+      <c r="L20" s="98"/>
+      <c r="M20" s="98">
+        <v>4</v>
+      </c>
+      <c r="N20" s="42"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
         <v>30</v>
       </c>
@@ -4613,23 +4715,24 @@
         <v>4</v>
       </c>
       <c r="F21" s="6"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="6">
+      <c r="G21" s="6"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="6">
         <v>6.2050000000000001</v>
       </c>
-      <c r="I21" s="98" t="s">
+      <c r="J21" s="98" t="s">
         <v>215</v>
       </c>
-      <c r="J21" s="98">
-        <v>6</v>
-      </c>
       <c r="K21" s="98">
-        <v>4</v>
-      </c>
-      <c r="L21" s="98"/>
-      <c r="M21" s="42"/>
-    </row>
-    <row r="22" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="L21" s="98">
+        <v>4</v>
+      </c>
+      <c r="M21" s="98"/>
+      <c r="N21" s="42"/>
+    </row>
+    <row r="22" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
         <v>30</v>
       </c>
@@ -4648,21 +4751,22 @@
       <c r="F22" s="6">
         <v>6</v>
       </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="6">
+      <c r="G22" s="6"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="6">
         <v>6.2050000000000001</v>
       </c>
-      <c r="I22" s="98" t="s">
+      <c r="J22" s="98" t="s">
         <v>216</v>
       </c>
-      <c r="J22" s="98">
-        <v>6</v>
-      </c>
-      <c r="K22" s="6"/>
+      <c r="K22" s="98">
+        <v>6</v>
+      </c>
       <c r="L22" s="6"/>
-      <c r="M22" s="42"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M22" s="6"/>
+      <c r="N22" s="42"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="38" t="s">
         <v>30</v>
       </c>
@@ -4677,23 +4781,24 @@
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="6">
+      <c r="G23" s="6"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="6">
         <v>6.2050000000000001</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="J23" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="J23" s="6">
-        <v>6</v>
-      </c>
       <c r="K23" s="6">
-        <v>4</v>
-      </c>
-      <c r="L23" s="6"/>
-      <c r="M23" s="42"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="L23" s="6">
+        <v>4</v>
+      </c>
+      <c r="M23" s="6"/>
+      <c r="N23" s="42"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="38" t="s">
         <v>30</v>
       </c>
@@ -4713,20 +4818,21 @@
         <v>6</v>
       </c>
       <c r="G24" s="8"/>
-      <c r="H24" s="6">
+      <c r="H24" s="8"/>
+      <c r="I24" s="6">
         <v>6.2050000000000001</v>
       </c>
-      <c r="I24" s="26" t="s">
+      <c r="J24" s="26" t="s">
         <v>289</v>
       </c>
-      <c r="J24" s="98"/>
       <c r="K24" s="98"/>
       <c r="L24" s="98"/>
-      <c r="M24" s="42" t="s">
+      <c r="M24" s="98"/>
+      <c r="N24" s="42" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="38" t="s">
         <v>30</v>
       </c>
@@ -4744,20 +4850,21 @@
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
-      <c r="H25" s="6">
+      <c r="H25" s="8"/>
+      <c r="I25" s="6">
         <v>6.2050000000000001</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="J25" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
-      <c r="M25" s="42" t="s">
+      <c r="M25" s="6"/>
+      <c r="N25" s="42" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="38" t="s">
         <v>30</v>
       </c>
@@ -4777,22 +4884,23 @@
         <v>8</v>
       </c>
       <c r="G26" s="8"/>
-      <c r="H26" s="6">
+      <c r="H26" s="8"/>
+      <c r="I26" s="6">
         <v>6.2050000000000001</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="J26" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="J26" s="6">
+      <c r="K26" s="6">
         <v>16</v>
       </c>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6">
+      <c r="L26" s="6"/>
+      <c r="M26" s="6">
         <v>0</v>
       </c>
-      <c r="M26" s="42"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" s="42"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="99" t="s">
         <v>30</v>
       </c>
@@ -4811,104 +4919,105 @@
       <c r="F27" s="101">
         <v>2</v>
       </c>
-      <c r="G27" s="100"/>
-      <c r="H27" s="100">
+      <c r="G27" s="101"/>
+      <c r="H27" s="100"/>
+      <c r="I27" s="100">
         <v>6.2050000000000001</v>
       </c>
-      <c r="I27" s="100" t="s">
+      <c r="J27" s="100" t="s">
         <v>300</v>
       </c>
-      <c r="J27" s="100"/>
       <c r="K27" s="100"/>
       <c r="L27" s="100"/>
-      <c r="M27" s="102"/>
-    </row>
-    <row r="102" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H102" s="14"/>
-    </row>
-    <row r="103" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H103" s="14"/>
-    </row>
-    <row r="105" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H105" s="14"/>
-    </row>
-    <row r="106" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H106" s="14"/>
-    </row>
-    <row r="107" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H107" s="14"/>
-    </row>
-    <row r="108" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H108" s="14"/>
-    </row>
-    <row r="109" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H109" s="14"/>
-    </row>
-    <row r="110" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H110" s="14"/>
-    </row>
-    <row r="111" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H111" s="14"/>
-    </row>
-    <row r="112" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H112" s="14"/>
-    </row>
-    <row r="113" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H113" s="14"/>
-    </row>
-    <row r="146" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H146" s="14"/>
-    </row>
-    <row r="147" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H147" s="14"/>
-    </row>
-    <row r="157" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H157" s="14"/>
-    </row>
-    <row r="158" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H158" s="14"/>
-    </row>
-    <row r="225" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H225" s="14"/>
-    </row>
-    <row r="226" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H226" s="14"/>
-    </row>
-    <row r="227" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H227" s="14"/>
-    </row>
-    <row r="228" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H228" s="14"/>
-    </row>
-    <row r="229" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H229" s="14"/>
-    </row>
-    <row r="230" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H230" s="14"/>
-    </row>
-    <row r="231" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H231" s="14"/>
-    </row>
-    <row r="232" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H232" s="14"/>
-    </row>
-    <row r="233" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H233" s="14"/>
-    </row>
-    <row r="234" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H234" s="14"/>
-    </row>
-    <row r="235" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H235" s="14"/>
-    </row>
-    <row r="236" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H236" s="14"/>
-    </row>
-    <row r="237" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H237" s="14"/>
-    </row>
-    <row r="238" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H238" s="14"/>
+      <c r="M27" s="100"/>
+      <c r="N27" s="102"/>
+    </row>
+    <row r="102" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I102" s="14"/>
+    </row>
+    <row r="103" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I103" s="14"/>
+    </row>
+    <row r="105" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I105" s="14"/>
+    </row>
+    <row r="106" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I106" s="14"/>
+    </row>
+    <row r="107" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I107" s="14"/>
+    </row>
+    <row r="108" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I108" s="14"/>
+    </row>
+    <row r="109" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I109" s="14"/>
+    </row>
+    <row r="110" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I110" s="14"/>
+    </row>
+    <row r="111" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I111" s="14"/>
+    </row>
+    <row r="112" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I112" s="14"/>
+    </row>
+    <row r="113" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I113" s="14"/>
+    </row>
+    <row r="146" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I146" s="14"/>
+    </row>
+    <row r="147" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I147" s="14"/>
+    </row>
+    <row r="157" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I157" s="14"/>
+    </row>
+    <row r="158" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I158" s="14"/>
+    </row>
+    <row r="225" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I225" s="14"/>
+    </row>
+    <row r="226" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I226" s="14"/>
+    </row>
+    <row r="227" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I227" s="14"/>
+    </row>
+    <row r="228" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I228" s="14"/>
+    </row>
+    <row r="229" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I229" s="14"/>
+    </row>
+    <row r="230" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I230" s="14"/>
+    </row>
+    <row r="231" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I231" s="14"/>
+    </row>
+    <row r="232" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I232" s="14"/>
+    </row>
+    <row r="233" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I233" s="14"/>
+    </row>
+    <row r="234" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I234" s="14"/>
+    </row>
+    <row r="235" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I235" s="14"/>
+    </row>
+    <row r="236" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I236" s="14"/>
+    </row>
+    <row r="237" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I237" s="14"/>
+    </row>
+    <row r="238" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I238" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Finished all except 7th grade
</commit_message>
<xml_diff>
--- a/Zaizd2.xlsx
+++ b/Zaizd2.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\rozklad\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="20730" windowHeight="9420" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="20730" windowHeight="9420" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1 курс" sheetId="1" r:id="rId1"/>
@@ -18,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'1 курс'!$A$1:$R$15</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -28,7 +33,7 @@
     <author>xgresx@gmail.com</author>
   </authors>
   <commentList>
-    <comment ref="N15" authorId="0">
+    <comment ref="N15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +58,7 @@
     <author>user</author>
   </authors>
   <commentList>
-    <comment ref="B24" authorId="0">
+    <comment ref="B24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +83,7 @@
     <author>xgresx@gmail.com</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N9" authorId="0">
+    <comment ref="N9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +124,7 @@
     <author>user</author>
   </authors>
   <commentList>
-    <comment ref="N25" authorId="0">
+    <comment ref="N25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -135,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B40" authorId="1">
+    <comment ref="B40" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -161,7 +166,7 @@
     <author>xgresx@gmail.com</author>
   </authors>
   <commentList>
-    <comment ref="B10" authorId="0">
+    <comment ref="B10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0">
+    <comment ref="B14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -191,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0">
+    <comment ref="B15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -217,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N18" authorId="1">
+    <comment ref="N18" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -242,7 +247,7 @@
     <author>user</author>
   </authors>
   <commentList>
-    <comment ref="B18" authorId="0">
+    <comment ref="B18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -257,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B34" authorId="0">
+    <comment ref="B34" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -277,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="332">
   <si>
     <t>Групи</t>
   </si>
@@ -1278,7 +1283,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1863,336 +1868,13 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Ввід" xfId="3" builtinId="20"/>
-    <cellStyle name="Добре" xfId="1" builtinId="26"/>
+    <cellStyle name="Гарний" xfId="1" builtinId="26"/>
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
+    <cellStyle name="Нейтральний" xfId="2" builtinId="28"/>
     <cellStyle name="Поганий" xfId="4" builtinId="27"/>
     <cellStyle name="Примітка" xfId="5" builtinId="10"/>
-    <cellStyle name="Середній" xfId="2" builtinId="28"/>
   </cellStyles>
-  <dxfs count="147">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="150">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -3360,6 +3042,81 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -3697,6 +3454,81 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -4011,6 +3843,81 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -4427,6 +4334,104 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -4852,6 +4857,81 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -5121,22 +5201,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:R27" totalsRowShown="0" headerRowDxfId="146" dataDxfId="144" headerRowBorderDxfId="145" tableBorderDxfId="143" totalsRowBorderDxfId="142">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:R27" totalsRowShown="0" headerRowDxfId="149" dataDxfId="147" headerRowBorderDxfId="148" tableBorderDxfId="146" totalsRowBorderDxfId="145">
   <autoFilter ref="A1:R27"/>
   <tableColumns count="18">
-    <tableColumn id="1" name="Групи" dataDxfId="141"/>
-    <tableColumn id="2" name="Дисципліна" dataDxfId="140"/>
-    <tableColumn id="3" name="Годин 1 заїзд" dataDxfId="139"/>
-    <tableColumn id="6" name="Годин 2 заїзд" dataDxfId="138"/>
-    <tableColumn id="14" name="Годин 3 заїзд" dataDxfId="137"/>
-    <tableColumn id="5" name="Годин 4 заїзд" dataDxfId="136"/>
-    <tableColumn id="15" name="Використано годин" dataDxfId="135"/>
-    <tableColumn id="17" name="Необхідно використати" dataDxfId="134">
+    <tableColumn id="1" name="Групи" dataDxfId="144"/>
+    <tableColumn id="2" name="Дисципліна" dataDxfId="143"/>
+    <tableColumn id="3" name="Годин 1 заїзд" dataDxfId="142"/>
+    <tableColumn id="6" name="Годин 2 заїзд" dataDxfId="141"/>
+    <tableColumn id="14" name="Годин 3 заїзд" dataDxfId="140"/>
+    <tableColumn id="5" name="Годин 4 заїзд" dataDxfId="139"/>
+    <tableColumn id="15" name="Використано годин" dataDxfId="138"/>
+    <tableColumn id="17" name="Необхідно використати" dataDxfId="137">
       <calculatedColumnFormula>Таблица1[[#This Row],[Годин 2 заїзд]]-Таблица1[[#This Row],[Використано годин]]+Таблица1[[#This Row],[Годин 1 заїзд]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Курс робота/проект" dataDxfId="15"/>
-    <tableColumn id="18" name="Іспит" dataDxfId="14"/>
-    <tableColumn id="20" name="Залік" dataDxfId="13"/>
+    <tableColumn id="16" name="Курс робота/проект" dataDxfId="136"/>
+    <tableColumn id="18" name="Іспит" dataDxfId="135"/>
+    <tableColumn id="20" name="Залік" dataDxfId="134"/>
     <tableColumn id="7" name="Прим." dataDxfId="133"/>
     <tableColumn id="8" name="шифр спеціальності" dataDxfId="132"/>
     <tableColumn id="9" name="Викладач" dataDxfId="131"/>
@@ -5163,147 +5243,150 @@
     <tableColumn id="3" name="Необхідно використати" dataDxfId="114">
       <calculatedColumnFormula>Таблица2[[#This Row],[Годин 1 заїзд]]+Таблица2[[#This Row],[Годин 2 заїзд]]-Таблица2[[#This Row],[Використано годин]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Курс робота/проект" dataDxfId="9"/>
-    <tableColumn id="18" name="Іспит" dataDxfId="10"/>
-    <tableColumn id="17" name="Залік" dataDxfId="11"/>
-    <tableColumn id="7" name="Прим." dataDxfId="12"/>
-    <tableColumn id="8" name="шифр спеціальності" dataDxfId="113"/>
-    <tableColumn id="9" name="Викладач" dataDxfId="112"/>
-    <tableColumn id="10" name="Лекц.2" dataDxfId="111"/>
-    <tableColumn id="11" name="Практ.3" dataDxfId="110"/>
-    <tableColumn id="12" name="Лаб." dataDxfId="109"/>
-    <tableColumn id="13" name="Столбец4" dataDxfId="108"/>
+    <tableColumn id="19" name="Курс робота/проект" dataDxfId="113"/>
+    <tableColumn id="18" name="Іспит" dataDxfId="112"/>
+    <tableColumn id="17" name="Залік" dataDxfId="111"/>
+    <tableColumn id="7" name="Прим." dataDxfId="110"/>
+    <tableColumn id="8" name="шифр спеціальності" dataDxfId="109"/>
+    <tableColumn id="9" name="Викладач" dataDxfId="108"/>
+    <tableColumn id="10" name="Лекц.2" dataDxfId="107"/>
+    <tableColumn id="11" name="Практ.3" dataDxfId="106"/>
+    <tableColumn id="12" name="Лаб." dataDxfId="105"/>
+    <tableColumn id="13" name="Столбец4" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Таблица3" displayName="Таблица3" ref="A1:Q44" totalsRowShown="0" headerRowDxfId="107" dataDxfId="105" headerRowBorderDxfId="106" tableBorderDxfId="104" totalsRowBorderDxfId="103">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Таблица3" displayName="Таблица3" ref="A1:Q44" totalsRowShown="0" headerRowDxfId="103" dataDxfId="101" headerRowBorderDxfId="102" tableBorderDxfId="100" totalsRowBorderDxfId="99">
   <autoFilter ref="A1:Q44"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Групи" dataDxfId="102"/>
-    <tableColumn id="2" name="Дисципліна" dataDxfId="101"/>
-    <tableColumn id="6" name="Годин 1 заїзд" dataDxfId="100"/>
-    <tableColumn id="14" name="Годин 2 заїзд" dataDxfId="99"/>
-    <tableColumn id="13" name="Годин 3 заїзд" dataDxfId="98"/>
-    <tableColumn id="5" name="Годин 4 заїзд" dataDxfId="97"/>
-    <tableColumn id="4" name="Використано годин" dataDxfId="96"/>
-    <tableColumn id="3" name="Необхідно використати" dataDxfId="95">
+    <tableColumn id="1" name="Групи" dataDxfId="98"/>
+    <tableColumn id="2" name="Дисципліна" dataDxfId="97"/>
+    <tableColumn id="6" name="Годин 1 заїзд" dataDxfId="96"/>
+    <tableColumn id="14" name="Годин 2 заїзд" dataDxfId="95"/>
+    <tableColumn id="13" name="Годин 3 заїзд" dataDxfId="94"/>
+    <tableColumn id="5" name="Годин 4 заїзд" dataDxfId="93"/>
+    <tableColumn id="4" name="Використано годин" dataDxfId="92"/>
+    <tableColumn id="3" name="Необхідно використати" dataDxfId="91">
       <calculatedColumnFormula>Таблица3[[#This Row],[Годин 1 заїзд]]+Таблица3[[#This Row],[Годин 2 заїзд]]-Таблица3[[#This Row],[Використано годин]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Курс робота/проект" dataDxfId="6"/>
-    <tableColumn id="16" name="Іспит" dataDxfId="7"/>
-    <tableColumn id="15" name="Залік" dataDxfId="8"/>
-    <tableColumn id="7" name="Прим." dataDxfId="94"/>
-    <tableColumn id="8" name="Шифр спеціальності" dataDxfId="93"/>
-    <tableColumn id="9" name="Викладач" dataDxfId="92"/>
-    <tableColumn id="10" name="Лекц.2" dataDxfId="91"/>
-    <tableColumn id="11" name="Практ.3" dataDxfId="90"/>
-    <tableColumn id="12" name="Лаб." dataDxfId="89"/>
+    <tableColumn id="17" name="Курс робота/проект" dataDxfId="90"/>
+    <tableColumn id="16" name="Іспит" dataDxfId="89"/>
+    <tableColumn id="15" name="Залік" dataDxfId="88"/>
+    <tableColumn id="7" name="Прим." dataDxfId="87"/>
+    <tableColumn id="8" name="Шифр спеціальності" dataDxfId="86"/>
+    <tableColumn id="9" name="Викладач" dataDxfId="85"/>
+    <tableColumn id="10" name="Лекц.2" dataDxfId="84"/>
+    <tableColumn id="11" name="Практ.3" dataDxfId="83"/>
+    <tableColumn id="12" name="Лаб." dataDxfId="82"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Таблица4" displayName="Таблица4" ref="A1:Q42" totalsRowShown="0" headerRowDxfId="88" dataDxfId="86" headerRowBorderDxfId="87" tableBorderDxfId="85" totalsRowBorderDxfId="84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Таблица4" displayName="Таблица4" ref="A1:Q42" totalsRowShown="0" headerRowDxfId="81" dataDxfId="79" headerRowBorderDxfId="80" tableBorderDxfId="78" totalsRowBorderDxfId="77">
   <autoFilter ref="A1:Q42"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Групи" dataDxfId="83"/>
-    <tableColumn id="2" name="Дисципліна" dataDxfId="82"/>
-    <tableColumn id="6" name="Годин 1 заїзд" dataDxfId="81"/>
-    <tableColumn id="13" name="Годин 2 заїзд" dataDxfId="80"/>
-    <tableColumn id="5" name="Годин 3 заїзд" dataDxfId="79"/>
-    <tableColumn id="4" name="Годин 4 заїзд" dataDxfId="78"/>
-    <tableColumn id="3" name="Використано годин" dataDxfId="77"/>
-    <tableColumn id="14" name="Необхідно використати" dataDxfId="76">
+    <tableColumn id="1" name="Групи" dataDxfId="76"/>
+    <tableColumn id="2" name="Дисципліна" dataDxfId="75"/>
+    <tableColumn id="6" name="Годин 1 заїзд" dataDxfId="74"/>
+    <tableColumn id="13" name="Годин 2 заїзд" dataDxfId="73"/>
+    <tableColumn id="5" name="Годин 3 заїзд" dataDxfId="72"/>
+    <tableColumn id="4" name="Годин 4 заїзд" dataDxfId="71"/>
+    <tableColumn id="3" name="Використано годин" dataDxfId="70"/>
+    <tableColumn id="14" name="Необхідно використати" dataDxfId="69">
       <calculatedColumnFormula>Таблица4[[#This Row],[Годин 1 заїзд]]+Таблица4[[#This Row],[Годин 2 заїзд]]-Таблица4[[#This Row],[Використано годин]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Курс робота/проект" dataDxfId="5"/>
-    <tableColumn id="16" name="Іспит" dataDxfId="4"/>
-    <tableColumn id="17" name="Залік" dataDxfId="3"/>
-    <tableColumn id="7" name="Прим." dataDxfId="75"/>
-    <tableColumn id="8" name="Шифр спеціальності" dataDxfId="74"/>
-    <tableColumn id="9" name="Викладач" dataDxfId="73"/>
-    <tableColumn id="10" name="Лекц.2" dataDxfId="72"/>
-    <tableColumn id="11" name="Практ.3" dataDxfId="71"/>
-    <tableColumn id="12" name="Лаб." dataDxfId="70"/>
+    <tableColumn id="15" name="Курс робота/проект" dataDxfId="68"/>
+    <tableColumn id="16" name="Іспит" dataDxfId="67"/>
+    <tableColumn id="17" name="Залік" dataDxfId="66"/>
+    <tableColumn id="7" name="Прим." dataDxfId="65"/>
+    <tableColumn id="8" name="Шифр спеціальності" dataDxfId="64"/>
+    <tableColumn id="9" name="Викладач" dataDxfId="63"/>
+    <tableColumn id="10" name="Лекц.2" dataDxfId="62"/>
+    <tableColumn id="11" name="Практ.3" dataDxfId="61"/>
+    <tableColumn id="12" name="Лаб." dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Таблица5" displayName="Таблица5" ref="A1:Q27" totalsRowShown="0" headerRowDxfId="69" dataDxfId="67" headerRowBorderDxfId="68" tableBorderDxfId="66" totalsRowBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Таблица5" displayName="Таблица5" ref="A1:Q27" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56" totalsRowBorderDxfId="55">
   <autoFilter ref="A1:Q27"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Групи" dataDxfId="64"/>
-    <tableColumn id="2" name="Дисципліна" dataDxfId="63"/>
-    <tableColumn id="6" name="Годин 1 заїзд" dataDxfId="62"/>
-    <tableColumn id="17" name="Годин 2 заїзд" dataDxfId="61"/>
-    <tableColumn id="16" name="Годин 3 заїзд" dataDxfId="60"/>
-    <tableColumn id="15" name="Годин 4 заїзд" dataDxfId="59"/>
-    <tableColumn id="14" name="Використано годин" dataDxfId="58"/>
-    <tableColumn id="13" name="Курс робота/проект" dataDxfId="0"/>
-    <tableColumn id="5" name="Іспит" dataDxfId="1"/>
-    <tableColumn id="4" name="Залік" dataDxfId="2"/>
-    <tableColumn id="3" name="Необхідно використати" dataDxfId="57">
+    <tableColumn id="1" name="Групи" dataDxfId="54"/>
+    <tableColumn id="2" name="Дисципліна" dataDxfId="53"/>
+    <tableColumn id="6" name="Годин 1 заїзд" dataDxfId="52"/>
+    <tableColumn id="17" name="Годин 2 заїзд" dataDxfId="51"/>
+    <tableColumn id="16" name="Годин 3 заїзд" dataDxfId="50"/>
+    <tableColumn id="15" name="Годин 4 заїзд" dataDxfId="49"/>
+    <tableColumn id="14" name="Використано годин" dataDxfId="48"/>
+    <tableColumn id="13" name="Курс робота/проект" dataDxfId="47"/>
+    <tableColumn id="5" name="Іспит" dataDxfId="46"/>
+    <tableColumn id="4" name="Залік" dataDxfId="45"/>
+    <tableColumn id="3" name="Необхідно використати" dataDxfId="44">
       <calculatedColumnFormula>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Прим." dataDxfId="56"/>
-    <tableColumn id="8" name="Шифр спецільності" dataDxfId="55"/>
-    <tableColumn id="9" name="Викладач" dataDxfId="54"/>
-    <tableColumn id="10" name="Лекц.2" dataDxfId="53"/>
-    <tableColumn id="11" name="Практ.3" dataDxfId="52"/>
-    <tableColumn id="12" name="Лаб." dataDxfId="51"/>
+    <tableColumn id="7" name="Прим." dataDxfId="43"/>
+    <tableColumn id="8" name="Шифр спецільності" dataDxfId="42"/>
+    <tableColumn id="9" name="Викладач" dataDxfId="41"/>
+    <tableColumn id="10" name="Лекц.2" dataDxfId="40"/>
+    <tableColumn id="11" name="Практ.3" dataDxfId="39"/>
+    <tableColumn id="12" name="Лаб." dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Таблица6" displayName="Таблица6" ref="A1:N48" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" tableBorderDxfId="48">
-  <autoFilter ref="A1:N48"/>
-  <tableColumns count="14">
-    <tableColumn id="1" name="Групи" dataDxfId="47"/>
-    <tableColumn id="2" name="Дисципліна" dataDxfId="46"/>
-    <tableColumn id="6" name="Годин 1 заїзд" dataDxfId="45"/>
-    <tableColumn id="13" name="Годин 2 заїзд" dataDxfId="44"/>
-    <tableColumn id="5" name="Годин 3 заїзд" dataDxfId="43"/>
-    <tableColumn id="4" name="Годин 4 заїзд" dataDxfId="42"/>
-    <tableColumn id="3" name="Використано годин" dataDxfId="41"/>
-    <tableColumn id="14" name="Необхідно використати" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Таблица6" displayName="Таблица6" ref="A1:Q48" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" tableBorderDxfId="35">
+  <autoFilter ref="A1:Q48"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="Групи" dataDxfId="34"/>
+    <tableColumn id="2" name="Дисципліна" dataDxfId="33"/>
+    <tableColumn id="6" name="Годин 1 заїзд" dataDxfId="32"/>
+    <tableColumn id="13" name="Годин 2 заїзд" dataDxfId="31"/>
+    <tableColumn id="5" name="Годин 3 заїзд" dataDxfId="30"/>
+    <tableColumn id="4" name="Годин 4 заїзд" dataDxfId="29"/>
+    <tableColumn id="3" name="Використано годин" dataDxfId="28"/>
+    <tableColumn id="14" name="Необхідно використати" dataDxfId="27">
       <calculatedColumnFormula>Таблица6[[#This Row],[Годин 1 заїзд]]+Таблица6[[#This Row],[Годин 2 заїзд]]+-Таблица6[[#This Row],[Використано годин]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Прим." dataDxfId="39"/>
-    <tableColumn id="8" name="Шифр. Спеціальності" dataDxfId="38"/>
-    <tableColumn id="9" name="Викладач" dataDxfId="37"/>
-    <tableColumn id="10" name="Лекц.2" dataDxfId="36"/>
-    <tableColumn id="11" name="Практ.3" dataDxfId="35"/>
-    <tableColumn id="12" name="Лаб." dataDxfId="34"/>
+    <tableColumn id="17" name="Курс робота/проект" dataDxfId="0"/>
+    <tableColumn id="16" name="Іспит" dataDxfId="1"/>
+    <tableColumn id="15" name="Залік" dataDxfId="2"/>
+    <tableColumn id="7" name="Прим." dataDxfId="26"/>
+    <tableColumn id="8" name="Шифр. Спеціальності" dataDxfId="25"/>
+    <tableColumn id="9" name="Викладач" dataDxfId="24"/>
+    <tableColumn id="10" name="Лекц.2" dataDxfId="23"/>
+    <tableColumn id="11" name="Практ.3" dataDxfId="22"/>
+    <tableColumn id="12" name="Лаб." dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Таблица7" displayName="Таблица7" ref="A1:M4" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Таблица7" displayName="Таблица7" ref="A1:M4" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="A1:M4"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Групи" dataDxfId="28"/>
-    <tableColumn id="2" name="Дисципліна" dataDxfId="27"/>
-    <tableColumn id="6" name="Годин 1 заїзд" dataDxfId="26"/>
-    <tableColumn id="13" name="Годин 2 заїзд" dataDxfId="25"/>
-    <tableColumn id="5" name="Годин 3 заїзд" dataDxfId="24"/>
-    <tableColumn id="4" name="Годин 4 заїзд" dataDxfId="23"/>
-    <tableColumn id="3" name="Використано годин" dataDxfId="22"/>
-    <tableColumn id="7" name="Прим." dataDxfId="21"/>
-    <tableColumn id="8" name="Шифр спецільності" dataDxfId="20"/>
-    <tableColumn id="9" name="Викладач" dataDxfId="19"/>
-    <tableColumn id="10" name="Лекц.2" dataDxfId="18"/>
-    <tableColumn id="11" name="Практ.3" dataDxfId="17"/>
-    <tableColumn id="12" name="Лаб." dataDxfId="16"/>
+    <tableColumn id="1" name="Групи" dataDxfId="15"/>
+    <tableColumn id="2" name="Дисципліна" dataDxfId="14"/>
+    <tableColumn id="6" name="Годин 1 заїзд" dataDxfId="13"/>
+    <tableColumn id="13" name="Годин 2 заїзд" dataDxfId="12"/>
+    <tableColumn id="5" name="Годин 3 заїзд" dataDxfId="11"/>
+    <tableColumn id="4" name="Годин 4 заїзд" dataDxfId="10"/>
+    <tableColumn id="3" name="Використано годин" dataDxfId="9"/>
+    <tableColumn id="7" name="Прим." dataDxfId="8"/>
+    <tableColumn id="8" name="Шифр спецільності" dataDxfId="7"/>
+    <tableColumn id="9" name="Викладач" dataDxfId="6"/>
+    <tableColumn id="10" name="Лекц.2" dataDxfId="5"/>
+    <tableColumn id="11" name="Практ.3" dataDxfId="4"/>
+    <tableColumn id="12" name="Лаб." dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5312,7 +5395,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Стандартна">
+    <a:clrScheme name="Офіс">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5350,9 +5433,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартна">
+    <a:fontScheme name="Офіс">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5387,7 +5470,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5422,7 +5505,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартна">
+    <a:fmtScheme name="Офіс">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5598,7 +5681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R238"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="I1" sqref="I1:K1"/>
     </sheetView>
   </sheetViews>
@@ -6915,7 +6998,7 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6924,8 +7007,8 @@
     <col min="2" max="2" width="61.7109375" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" style="29" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="29" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="29" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="29" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="29" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="29" hidden="1" customWidth="1"/>
     <col min="7" max="8" width="14.28515625" style="29" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" style="29" customWidth="1"/>
     <col min="10" max="10" width="7.140625" style="29" customWidth="1"/>
@@ -7877,7 +7960,9 @@
         <v>4</v>
       </c>
       <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="J22" s="4">
+        <v>4</v>
+      </c>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4">
@@ -7918,7 +8003,9 @@
         <v>6</v>
       </c>
       <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
+      <c r="J23" s="4">
+        <v>2</v>
+      </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4">
@@ -7963,7 +8050,9 @@
         <v>8</v>
       </c>
       <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
+      <c r="J24" s="4">
+        <v>4</v>
+      </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4">
@@ -8004,7 +8093,9 @@
         <v>6</v>
       </c>
       <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
+      <c r="J25" s="4">
+        <v>4</v>
+      </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4">
@@ -8044,7 +8135,9 @@
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
+      <c r="K26" s="4">
+        <v>2</v>
+      </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4">
         <v>6.090103</v>
@@ -8086,7 +8179,9 @@
         <v>6</v>
       </c>
       <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
+      <c r="J27" s="4">
+        <v>4</v>
+      </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4">
@@ -8129,7 +8224,9 @@
         <v>4</v>
       </c>
       <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
+      <c r="J28" s="4">
+        <v>4</v>
+      </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4">
@@ -8171,7 +8268,9 @@
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+      <c r="K29" s="4">
+        <v>3</v>
+      </c>
       <c r="L29" s="4"/>
       <c r="M29" s="4">
         <v>6.090103</v>
@@ -8215,7 +8314,9 @@
         <v>6</v>
       </c>
       <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="J30" s="4">
+        <v>4</v>
+      </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4">
@@ -8260,7 +8361,9 @@
         <v>6</v>
       </c>
       <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
+      <c r="J31" s="4">
+        <v>3</v>
+      </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4">
@@ -8303,7 +8406,9 @@
         <v>6</v>
       </c>
       <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
+      <c r="J32" s="22">
+        <v>3</v>
+      </c>
       <c r="K32" s="22"/>
       <c r="L32" s="22"/>
       <c r="M32" s="22">
@@ -8335,16 +8440,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="14.28515625" style="7" customWidth="1"/>
-    <col min="6" max="7" width="10.7109375" style="7" customWidth="1"/>
+    <col min="3" max="4" width="14.28515625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="7" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="7" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="7" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" style="7" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="7" customWidth="1"/>
     <col min="10" max="10" width="7.42578125" style="7" customWidth="1"/>
@@ -9344,7 +9451,9 @@
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="K24" s="4">
+        <v>3</v>
+      </c>
       <c r="L24" s="4"/>
       <c r="M24" s="4">
         <v>6.080101</v>
@@ -9385,7 +9494,9 @@
         <v>4</v>
       </c>
       <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
+      <c r="J25" s="4">
+        <v>4</v>
+      </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4">
@@ -9424,7 +9535,9 @@
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
+      <c r="K26" s="4">
+        <v>2</v>
+      </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4">
         <v>6.080101</v>
@@ -9464,7 +9577,9 @@
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
+      <c r="K27" s="4">
+        <v>3</v>
+      </c>
       <c r="L27" s="4"/>
       <c r="M27" s="4">
         <v>6.080101</v>
@@ -9503,7 +9618,9 @@
         <v>6</v>
       </c>
       <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
+      <c r="J28" s="4">
+        <v>2</v>
+      </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4">
@@ -9543,7 +9660,9 @@
         <v>0</v>
       </c>
       <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
+      <c r="J29" s="4">
+        <v>4</v>
+      </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4">
@@ -9580,8 +9699,12 @@
         <f>Таблица3[[#This Row],[Годин 1 заїзд]]+Таблица3[[#This Row],[Годин 2 заїзд]]-Таблица3[[#This Row],[Використано годин]]</f>
         <v>6</v>
       </c>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="I30" s="4">
+        <v>4</v>
+      </c>
+      <c r="J30" s="4">
+        <v>4</v>
+      </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4">
@@ -9622,7 +9745,9 @@
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
+      <c r="K31" s="4">
+        <v>2</v>
+      </c>
       <c r="L31" s="4" t="s">
         <v>200</v>
       </c>
@@ -9661,7 +9786,9 @@
         <v>4</v>
       </c>
       <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
+      <c r="J32" s="4">
+        <v>4</v>
+      </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4">
@@ -9703,7 +9830,9 @@
         <v>4</v>
       </c>
       <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
+      <c r="J33" s="4">
+        <v>4</v>
+      </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4">
@@ -9744,7 +9873,9 @@
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
+      <c r="K34" s="4">
+        <v>2</v>
+      </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4">
         <v>6.090103</v>
@@ -9782,8 +9913,12 @@
         <f>Таблица3[[#This Row],[Годин 1 заїзд]]+Таблица3[[#This Row],[Годин 2 заїзд]]-Таблица3[[#This Row],[Використано годин]]</f>
         <v>6</v>
       </c>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
+      <c r="I35" s="4">
+        <v>3</v>
+      </c>
+      <c r="J35" s="4">
+        <v>4</v>
+      </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4">
@@ -9825,7 +9960,9 @@
         <v>4</v>
       </c>
       <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
+      <c r="J36" s="4">
+        <v>3</v>
+      </c>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4">
@@ -9866,7 +10003,9 @@
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
+      <c r="K37" s="4">
+        <v>2</v>
+      </c>
       <c r="L37" s="4"/>
       <c r="M37" s="4">
         <v>6.090103</v>
@@ -9908,7 +10047,9 @@
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
+      <c r="K38" s="4">
+        <v>3</v>
+      </c>
       <c r="L38" s="4"/>
       <c r="M38" s="4">
         <v>6.090103</v>
@@ -9945,7 +10086,9 @@
         <v>6</v>
       </c>
       <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
+      <c r="J39" s="4">
+        <v>3</v>
+      </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4">
@@ -9987,7 +10130,9 @@
         <v>6</v>
       </c>
       <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
+      <c r="J40" s="4">
+        <v>3</v>
+      </c>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4">
@@ -10023,7 +10168,9 @@
         <v>4</v>
       </c>
       <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
+      <c r="J41" s="4">
+        <v>3</v>
+      </c>
       <c r="K41" s="4"/>
       <c r="L41" s="4" t="s">
         <v>201</v>
@@ -10061,7 +10208,9 @@
         <v>4</v>
       </c>
       <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
+      <c r="J42" s="4">
+        <v>3</v>
+      </c>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4">
@@ -10106,7 +10255,9 @@
       </c>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
+      <c r="K43" s="4">
+        <v>4</v>
+      </c>
       <c r="L43" s="4"/>
       <c r="M43" s="4">
         <v>6.090103</v>
@@ -10150,7 +10301,9 @@
       </c>
       <c r="I44" s="22"/>
       <c r="J44" s="22"/>
-      <c r="K44" s="22"/>
+      <c r="K44" s="22">
+        <v>4</v>
+      </c>
       <c r="L44" s="22"/>
       <c r="M44" s="22">
         <v>6.090103</v>
@@ -10343,15 +10496,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:K1"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="14.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="14.28515625" style="6" customWidth="1"/>
+    <col min="5" max="6" width="14.28515625" style="6" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="6" customWidth="1"/>
     <col min="8" max="8" width="9" style="6" customWidth="1"/>
     <col min="9" max="9" width="8.5703125" style="6" customWidth="1"/>
     <col min="10" max="11" width="6.28515625" style="6" customWidth="1"/>
@@ -11012,7 +11167,9 @@
         <v>4</v>
       </c>
       <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
+      <c r="J16" s="4">
+        <v>4</v>
+      </c>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4">
@@ -11052,7 +11209,9 @@
         <v>0</v>
       </c>
       <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="J17" s="4">
+        <v>4</v>
+      </c>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4">
@@ -11090,7 +11249,9 @@
         <v>4</v>
       </c>
       <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
+      <c r="J18" s="4">
+        <v>3</v>
+      </c>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4">
@@ -11129,7 +11290,9 @@
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
+      <c r="K19" s="4">
+        <v>4</v>
+      </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4">
         <v>6.080101</v>
@@ -11169,7 +11332,9 @@
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
+      <c r="K20" s="4">
+        <v>4</v>
+      </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4">
         <v>6.080101</v>
@@ -11205,7 +11370,9 @@
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
+      <c r="K21" s="4">
+        <v>2</v>
+      </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4">
         <v>6.080101</v>
@@ -11244,7 +11411,9 @@
         <v>2</v>
       </c>
       <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="J22" s="4">
+        <v>2</v>
+      </c>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4">
@@ -11285,7 +11454,9 @@
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
+      <c r="K23" s="4">
+        <v>2</v>
+      </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4">
         <v>6.080101</v>
@@ -11325,7 +11496,9 @@
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="K24" s="4">
+        <v>2</v>
+      </c>
       <c r="L24" s="4"/>
       <c r="M24" s="4">
         <v>6.080101</v>
@@ -11362,7 +11535,9 @@
         <v>0</v>
       </c>
       <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
+      <c r="J25" s="41">
+        <v>4</v>
+      </c>
       <c r="K25" s="41"/>
       <c r="L25" s="41"/>
       <c r="M25" s="41">
@@ -11404,7 +11579,9 @@
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
+      <c r="K26" s="4">
+        <v>4</v>
+      </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4">
         <v>6.080101</v>
@@ -11444,7 +11621,9 @@
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
+      <c r="K27" s="4">
+        <v>4</v>
+      </c>
       <c r="L27" s="4"/>
       <c r="M27" s="4">
         <v>6.080101</v>
@@ -11479,7 +11658,9 @@
         <v>6</v>
       </c>
       <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
+      <c r="J28" s="4">
+        <v>3</v>
+      </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4">
@@ -11518,7 +11699,9 @@
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+      <c r="K29" s="4">
+        <v>3</v>
+      </c>
       <c r="L29" s="4"/>
       <c r="M29" s="4">
         <v>6.080101</v>
@@ -11551,7 +11734,9 @@
         <v>4</v>
       </c>
       <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="J30" s="4">
+        <v>3</v>
+      </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4" t="s">
         <v>201</v>
@@ -11588,7 +11773,9 @@
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
+      <c r="K31" s="4">
+        <v>2</v>
+      </c>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="3"/>
@@ -11622,7 +11809,9 @@
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
+      <c r="K32" s="4">
+        <v>3</v>
+      </c>
       <c r="L32" s="4"/>
       <c r="M32" s="4">
         <v>6.090103</v>
@@ -11665,7 +11854,9 @@
         <v>4</v>
       </c>
       <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
+      <c r="J33" s="4">
+        <v>4</v>
+      </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4">
@@ -11709,7 +11900,9 @@
         <v>8</v>
       </c>
       <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
+      <c r="J34" s="4">
+        <v>4</v>
+      </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4">
@@ -11751,7 +11944,9 @@
         <v>4</v>
       </c>
       <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
+      <c r="J35" s="4">
+        <v>3</v>
+      </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4">
@@ -11793,7 +11988,9 @@
         <v>4</v>
       </c>
       <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
+      <c r="J36" s="4">
+        <v>3</v>
+      </c>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4">
@@ -11836,7 +12033,9 @@
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
+      <c r="K37" s="4">
+        <v>4</v>
+      </c>
       <c r="L37" s="4"/>
       <c r="M37" s="4">
         <v>6.090103</v>
@@ -11878,7 +12077,9 @@
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
+      <c r="K38" s="4">
+        <v>3</v>
+      </c>
       <c r="L38" s="4"/>
       <c r="M38" s="4">
         <v>6.090103</v>
@@ -11917,7 +12118,9 @@
         <v>2</v>
       </c>
       <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
+      <c r="J39" s="4">
+        <v>4</v>
+      </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4">
@@ -11960,9 +12163,13 @@
         <f>Таблица4[[#This Row],[Годин 1 заїзд]]+Таблица4[[#This Row],[Годин 2 заїзд]]-Таблица4[[#This Row],[Використано годин]]</f>
         <v>4</v>
       </c>
-      <c r="I40" s="4"/>
+      <c r="I40" s="4">
+        <v>3</v>
+      </c>
       <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
+      <c r="K40" s="4">
+        <v>4</v>
+      </c>
       <c r="L40" s="4"/>
       <c r="M40" s="4">
         <v>6.090103</v>
@@ -12000,7 +12207,9 @@
         <f>Таблица4[[#This Row],[Годин 1 заїзд]]+Таблица4[[#This Row],[Годин 2 заїзд]]-Таблица4[[#This Row],[Використано годин]]</f>
         <v>4</v>
       </c>
-      <c r="I41" s="4"/>
+      <c r="I41" s="4">
+        <v>3</v>
+      </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
@@ -12044,7 +12253,9 @@
       </c>
       <c r="I42" s="22"/>
       <c r="J42" s="22"/>
-      <c r="K42" s="22"/>
+      <c r="K42" s="22">
+        <v>3</v>
+      </c>
       <c r="L42" s="22"/>
       <c r="M42" s="22">
         <v>6.090103</v>
@@ -12073,15 +12284,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="7" customWidth="1"/>
     <col min="2" max="2" width="51.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="14.28515625" style="7" customWidth="1"/>
+    <col min="3" max="4" width="14.28515625" style="7" customWidth="1"/>
+    <col min="5" max="6" width="14.28515625" style="7" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="7" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" style="7" customWidth="1"/>
     <col min="9" max="9" width="6" style="7" customWidth="1"/>
     <col min="10" max="10" width="8.5703125" style="7" customWidth="1"/>
@@ -12515,7 +12728,9 @@
         <v>10</v>
       </c>
       <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="4">
+        <v>3</v>
+      </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
@@ -12557,7 +12772,9 @@
         <v>8</v>
       </c>
       <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="I11" s="4">
+        <v>3</v>
+      </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
@@ -12600,7 +12817,9 @@
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
+      <c r="J12" s="4">
+        <v>3</v>
+      </c>
       <c r="K12" s="4">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
         <v>10</v>
@@ -12640,7 +12859,9 @@
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="J13" s="4">
+        <v>2</v>
+      </c>
       <c r="K13" s="4">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
         <v>4</v>
@@ -12678,7 +12899,9 @@
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+      <c r="J14" s="4">
+        <v>2</v>
+      </c>
       <c r="K14" s="4">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
         <v>12</v>
@@ -12714,7 +12937,9 @@
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="J15" s="4">
+        <v>2</v>
+      </c>
       <c r="K15" s="4">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
         <v>6</v>
@@ -12754,7 +12979,9 @@
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
+      <c r="J16" s="4">
+        <v>2</v>
+      </c>
       <c r="K16" s="4">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
         <v>4</v>
@@ -12795,7 +13022,9 @@
         <v>8</v>
       </c>
       <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="I17" s="4">
+        <v>3</v>
+      </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
@@ -12837,7 +13066,9 @@
         <v>0</v>
       </c>
       <c r="H18" s="79"/>
-      <c r="I18" s="79"/>
+      <c r="I18" s="79">
+        <v>3</v>
+      </c>
       <c r="J18" s="79"/>
       <c r="K18" s="79">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
@@ -12876,7 +13107,9 @@
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="J19" s="4">
+        <v>3</v>
+      </c>
       <c r="K19" s="4">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
         <v>4</v>
@@ -12917,7 +13150,9 @@
         <v>8</v>
       </c>
       <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="I20" s="4">
+        <v>3</v>
+      </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
@@ -12959,7 +13194,9 @@
         <v>6</v>
       </c>
       <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="I21" s="4">
+        <v>3</v>
+      </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
@@ -13000,7 +13237,9 @@
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="J22" s="4">
+        <v>2</v>
+      </c>
       <c r="K22" s="4">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
         <v>6</v>
@@ -13038,7 +13277,9 @@
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
+      <c r="J23" s="4">
+        <v>3</v>
+      </c>
       <c r="K23" s="4">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
         <v>6</v>
@@ -13079,7 +13320,9 @@
         <v>4</v>
       </c>
       <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
+      <c r="I24" s="4">
+        <v>3</v>
+      </c>
       <c r="J24" s="4"/>
       <c r="K24" s="4">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
@@ -13117,7 +13360,9 @@
         <v>0</v>
       </c>
       <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
+      <c r="I25" s="4">
+        <v>3</v>
+      </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
@@ -13156,7 +13401,9 @@
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
+      <c r="J26" s="4">
+        <v>2</v>
+      </c>
       <c r="K26" s="4">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
         <v>2</v>
@@ -13192,7 +13439,9 @@
       </c>
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="J27" s="22">
+        <v>2</v>
+      </c>
       <c r="K27" s="22">
         <f>Таблица5[[#This Row],[Годин 1 заїзд]]+Таблица5[[#This Row],[Годин 2 заїзд]]+-Таблица5[[#This Row],[Використано годин]]</f>
         <v>4</v>
@@ -13223,27 +13472,32 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.85546875" style="49" customWidth="1"/>
-    <col min="3" max="8" width="14.28515625" style="48" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="48" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" style="48" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" style="48" customWidth="1"/>
-    <col min="13" max="13" width="10" style="48" customWidth="1"/>
-    <col min="14" max="14" width="7.140625" style="48" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="48"/>
+    <col min="2" max="2" width="52" style="49" customWidth="1"/>
+    <col min="3" max="4" width="14.28515625" style="48" customWidth="1"/>
+    <col min="5" max="6" width="14.28515625" style="48" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="14.28515625" style="48" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="48" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" style="48" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="48" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="48" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="48" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="23.85546875" style="48" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" style="48" customWidth="1"/>
+    <col min="16" max="16" width="10" style="48" customWidth="1"/>
+    <col min="17" max="17" width="7.140625" style="48" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -13268,26 +13522,35 @@
       <c r="H1" s="22" t="s">
         <v>326</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="L1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="M1" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="K1" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="21" t="s">
+      <c r="N1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>171</v>
       </c>
@@ -13310,19 +13573,24 @@
         <v>10</v>
       </c>
       <c r="I2" s="4"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3" t="s">
+      <c r="J2" s="4">
+        <v>2</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="L2" s="3">
+      <c r="O2" s="3">
         <v>16</v>
       </c>
-      <c r="M2" s="3">
-        <v>4</v>
-      </c>
-      <c r="N2" s="57"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P2" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="57"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>171</v>
       </c>
@@ -13344,20 +13612,27 @@
         <f>Таблица6[[#This Row],[Годин 1 заїзд]]+Таблица6[[#This Row],[Годин 2 заїзд]]+-Таблица6[[#This Row],[Використано годин]]</f>
         <v>10</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="3" t="s">
+      <c r="I3" s="4">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4">
+        <v>2</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="L3" s="3">
+      <c r="O3" s="3">
         <v>16</v>
       </c>
-      <c r="M3" s="3">
-        <v>4</v>
-      </c>
-      <c r="N3" s="57"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P3" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="57"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>171</v>
       </c>
@@ -13380,15 +13655,20 @@
         <v>2</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="3" t="s">
+      <c r="J4" s="4">
+        <v>2</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="57"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="57"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>170</v>
       </c>
@@ -13411,19 +13691,24 @@
         <v>4</v>
       </c>
       <c r="I5" s="77"/>
-      <c r="J5" s="77">
+      <c r="J5" s="77"/>
+      <c r="K5" s="77">
+        <v>2</v>
+      </c>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77">
         <v>7.0140000000000002</v>
       </c>
-      <c r="K5" s="76" t="s">
+      <c r="N5" s="76" t="s">
         <v>212</v>
       </c>
-      <c r="L5" s="76"/>
-      <c r="M5" s="76">
+      <c r="O5" s="76"/>
+      <c r="P5" s="76">
         <v>10</v>
       </c>
-      <c r="N5" s="81"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q5" s="81"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>170</v>
       </c>
@@ -13446,21 +13731,26 @@
         <v>6</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="4">
+      <c r="J6" s="4"/>
+      <c r="K6" s="4">
+        <v>2</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4">
         <v>7.0140000000000002</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="N6" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="L6" s="19">
+      <c r="O6" s="19">
         <v>12</v>
       </c>
-      <c r="M6" s="19">
-        <v>4</v>
-      </c>
-      <c r="N6" s="57"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P6" s="19">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="57"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>171</v>
       </c>
@@ -13483,17 +13773,22 @@
         <v>4</v>
       </c>
       <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="10" t="s">
+      <c r="J7" s="4">
+        <v>3</v>
+      </c>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="L7" s="10">
-        <v>4</v>
-      </c>
-      <c r="M7" s="3"/>
-      <c r="N7" s="57"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="10">
+        <v>4</v>
+      </c>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="57"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>171</v>
       </c>
@@ -13518,17 +13813,22 @@
         <v>6</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="3" t="s">
+      <c r="J8" s="4">
+        <v>3</v>
+      </c>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="L8" s="3">
+      <c r="O8" s="3">
         <v>14</v>
       </c>
-      <c r="M8" s="3"/>
-      <c r="N8" s="57"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P8" s="3"/>
+      <c r="Q8" s="57"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>171</v>
       </c>
@@ -13551,17 +13851,22 @@
         <v>4</v>
       </c>
       <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="3" t="s">
+      <c r="J9" s="4">
+        <v>3</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="L9" s="3">
-        <v>4</v>
-      </c>
-      <c r="M9" s="3"/>
-      <c r="N9" s="57"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="3">
+        <v>4</v>
+      </c>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="57"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>170</v>
       </c>
@@ -13584,19 +13889,24 @@
         <v>6</v>
       </c>
       <c r="I10" s="4"/>
-      <c r="J10" s="4">
+      <c r="J10" s="4"/>
+      <c r="K10" s="4">
+        <v>3</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4">
         <v>7.0140000000000002</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="N10" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="L10" s="10">
-        <v>6</v>
-      </c>
-      <c r="M10" s="3"/>
-      <c r="N10" s="57"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="10">
+        <v>6</v>
+      </c>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="57"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>171</v>
       </c>
@@ -13620,16 +13930,21 @@
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="19" t="s">
+      <c r="K11" s="4">
+        <v>3</v>
+      </c>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="L11" s="19">
-        <v>8</v>
-      </c>
-      <c r="M11" s="3"/>
-      <c r="N11" s="57"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="19">
+        <v>8</v>
+      </c>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="57"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>171</v>
       </c>
@@ -13651,16 +13966,23 @@
         <f>Таблица6[[#This Row],[Годин 1 заїзд]]+Таблица6[[#This Row],[Годин 2 заїзд]]+-Таблица6[[#This Row],[Використано годин]]</f>
         <v>0</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="3" t="s">
+      <c r="I12" s="4">
+        <v>4</v>
+      </c>
+      <c r="J12" s="4">
+        <v>4</v>
+      </c>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="57"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="57"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>171</v>
       </c>
@@ -13683,15 +14005,20 @@
         <v>0</v>
       </c>
       <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="10" t="s">
+      <c r="J13" s="4">
+        <v>4</v>
+      </c>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="57"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="57"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>171</v>
       </c>
@@ -13714,15 +14041,20 @@
         <v>0</v>
       </c>
       <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="10" t="s">
+      <c r="J14" s="4">
+        <v>4</v>
+      </c>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="57"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="57"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>171</v>
       </c>
@@ -13745,13 +14077,18 @@
         <v>0</v>
       </c>
       <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="57"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J15" s="4">
+        <v>4</v>
+      </c>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="57"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>179</v>
       </c>
@@ -13775,18 +14112,23 @@
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="10" t="s">
+      <c r="K16" s="4">
+        <v>2</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="L16" s="10">
-        <v>8</v>
-      </c>
-      <c r="M16" s="10">
-        <v>4</v>
-      </c>
-      <c r="N16" s="57"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="10">
+        <v>8</v>
+      </c>
+      <c r="P16" s="10">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="57"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>179</v>
       </c>
@@ -13810,18 +14152,23 @@
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="10" t="s">
+      <c r="K17" s="4">
+        <v>2</v>
+      </c>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="L17" s="10">
-        <v>8</v>
-      </c>
-      <c r="M17" s="10">
-        <v>4</v>
-      </c>
-      <c r="N17" s="57"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" s="10">
+        <v>8</v>
+      </c>
+      <c r="P17" s="10">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="57"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>179</v>
       </c>
@@ -13844,19 +14191,24 @@
         <v>14</v>
       </c>
       <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="10" t="s">
+      <c r="J18" s="4">
+        <v>2</v>
+      </c>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="L18" s="19">
-        <v>8</v>
-      </c>
-      <c r="M18" s="19">
-        <v>6</v>
-      </c>
-      <c r="N18" s="57"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="19">
+        <v>8</v>
+      </c>
+      <c r="P18" s="19">
+        <v>6</v>
+      </c>
+      <c r="Q18" s="57"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>179</v>
       </c>
@@ -13878,20 +14230,27 @@
         <f>Таблица6[[#This Row],[Годин 1 заїзд]]+Таблица6[[#This Row],[Годин 2 заїзд]]+-Таблица6[[#This Row],[Використано годин]]</f>
         <v>4</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="3" t="s">
+      <c r="I19" s="4">
+        <v>2</v>
+      </c>
+      <c r="J19" s="4">
+        <v>2</v>
+      </c>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="L19" s="3">
-        <v>8</v>
-      </c>
-      <c r="M19" s="3">
-        <v>4</v>
-      </c>
-      <c r="N19" s="57"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="3">
+        <v>8</v>
+      </c>
+      <c r="P19" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="57"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>179</v>
       </c>
@@ -13916,19 +14275,24 @@
         <v>8</v>
       </c>
       <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="10" t="s">
+      <c r="J20" s="4">
+        <v>3</v>
+      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="L20" s="19">
+      <c r="O20" s="19">
         <v>10</v>
       </c>
-      <c r="M20" s="19">
-        <v>4</v>
-      </c>
-      <c r="N20" s="57"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P20" s="19">
+        <v>4</v>
+      </c>
+      <c r="Q20" s="57"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>179</v>
       </c>
@@ -13953,19 +14317,24 @@
         <v>6</v>
       </c>
       <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="10" t="s">
+      <c r="J21" s="4">
+        <v>3</v>
+      </c>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="L21" s="10">
+      <c r="O21" s="10">
         <v>10</v>
       </c>
-      <c r="M21" s="10">
-        <v>2</v>
-      </c>
-      <c r="N21" s="57"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P21" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="57"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>179</v>
       </c>
@@ -13989,18 +14358,23 @@
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="10" t="s">
+      <c r="K22" s="4">
+        <v>2</v>
+      </c>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="L22" s="10">
-        <v>8</v>
-      </c>
-      <c r="M22" s="10">
-        <v>4</v>
-      </c>
-      <c r="N22" s="57"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22" s="10">
+        <v>8</v>
+      </c>
+      <c r="P22" s="10">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="57"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>179</v>
       </c>
@@ -14023,17 +14397,22 @@
         <v>6</v>
       </c>
       <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="10" t="s">
+      <c r="J23" s="4">
+        <v>3</v>
+      </c>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="L23" s="10">
-        <v>6</v>
-      </c>
-      <c r="M23" s="3"/>
-      <c r="N23" s="57"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23" s="10">
+        <v>6</v>
+      </c>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="57"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>180</v>
       </c>
@@ -14057,18 +14436,23 @@
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4">
+        <v>3</v>
+      </c>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4">
         <v>7.1929999999999996</v>
       </c>
-      <c r="K24" s="10" t="s">
+      <c r="N24" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="L24" s="10">
-        <v>6</v>
-      </c>
-      <c r="M24" s="3"/>
-      <c r="N24" s="57"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24" s="10">
+        <v>6</v>
+      </c>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="57"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>179</v>
       </c>
@@ -14092,16 +14476,21 @@
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
-      <c r="K25" s="10" t="s">
+      <c r="K25" s="4">
+        <v>2</v>
+      </c>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="L25" s="10">
-        <v>6</v>
-      </c>
-      <c r="M25" s="3"/>
-      <c r="N25" s="57"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25" s="10">
+        <v>6</v>
+      </c>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="57"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>179</v>
       </c>
@@ -14125,16 +14514,21 @@
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
-      <c r="K26" s="10" t="s">
+      <c r="K26" s="4">
+        <v>2</v>
+      </c>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="L26" s="10">
-        <v>8</v>
-      </c>
-      <c r="M26" s="3"/>
-      <c r="N26" s="57"/>
-    </row>
-    <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="O26" s="10">
+        <v>8</v>
+      </c>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="57"/>
+    </row>
+    <row r="27" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>179</v>
       </c>
@@ -14157,17 +14551,22 @@
         <v>8</v>
       </c>
       <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="31" t="s">
+      <c r="J27" s="4">
+        <v>3</v>
+      </c>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="31" t="s">
         <v>270</v>
       </c>
-      <c r="L27" s="10">
-        <v>8</v>
-      </c>
-      <c r="M27" s="3"/>
-      <c r="N27" s="57"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27" s="10">
+        <v>8</v>
+      </c>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="57"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>179</v>
       </c>
@@ -14191,18 +14590,23 @@
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
-      <c r="K28" s="10" t="s">
+      <c r="K28" s="4">
+        <v>2</v>
+      </c>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="L28" s="19">
-        <v>8</v>
-      </c>
-      <c r="M28" s="19">
-        <v>4</v>
-      </c>
-      <c r="N28" s="57"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28" s="19">
+        <v>8</v>
+      </c>
+      <c r="P28" s="19">
+        <v>4</v>
+      </c>
+      <c r="Q28" s="57"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>179</v>
       </c>
@@ -14225,15 +14629,20 @@
         <v>4</v>
       </c>
       <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="3" t="s">
+      <c r="J29" s="4">
+        <v>2</v>
+      </c>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="57"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="57"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>184</v>
       </c>
@@ -14256,19 +14665,24 @@
         <v>6</v>
       </c>
       <c r="I30" s="4"/>
-      <c r="J30" s="4">
+      <c r="J30" s="4"/>
+      <c r="K30" s="4">
+        <v>2</v>
+      </c>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4">
         <v>8.0139999999999993</v>
       </c>
-      <c r="K30" s="10" t="s">
+      <c r="N30" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10">
+      <c r="O30" s="10"/>
+      <c r="P30" s="10">
         <v>10</v>
       </c>
-      <c r="N30" s="57"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q30" s="57"/>
+    </row>
+    <row r="31" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>184</v>
       </c>
@@ -14291,19 +14705,24 @@
         <v>6</v>
       </c>
       <c r="I31" s="4"/>
-      <c r="J31" s="4">
+      <c r="J31" s="4"/>
+      <c r="K31" s="4">
+        <v>3</v>
+      </c>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4">
         <v>8.0139999999999993</v>
       </c>
-      <c r="K31" s="10" t="s">
+      <c r="N31" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="L31" s="10">
-        <v>6</v>
-      </c>
-      <c r="M31" s="3"/>
-      <c r="N31" s="57"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31" s="10">
+        <v>6</v>
+      </c>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="57"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>184</v>
       </c>
@@ -14327,16 +14746,21 @@
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4">
+        <v>4</v>
+      </c>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4">
         <v>8.0139999999999993</v>
       </c>
-      <c r="K32" s="10" t="s">
+      <c r="N32" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="L32" s="19"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="57"/>
-    </row>
-    <row r="33" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="O32" s="19"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="57"/>
+    </row>
+    <row r="33" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>186</v>
       </c>
@@ -14359,21 +14783,26 @@
         <v>6</v>
       </c>
       <c r="I33" s="4"/>
-      <c r="J33" s="4">
+      <c r="J33" s="4"/>
+      <c r="K33" s="4">
+        <v>3</v>
+      </c>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4">
         <v>8.1929999999999996</v>
       </c>
-      <c r="K33" s="10" t="s">
+      <c r="N33" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="L33" s="3">
-        <v>6</v>
-      </c>
-      <c r="M33" s="3">
+      <c r="O33" s="3">
+        <v>6</v>
+      </c>
+      <c r="P33" s="3">
         <v>0</v>
       </c>
-      <c r="N33" s="57"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q33" s="57"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>186</v>
       </c>
@@ -14398,21 +14827,26 @@
         <v>10</v>
       </c>
       <c r="I34" s="4"/>
-      <c r="J34" s="4">
+      <c r="J34" s="4"/>
+      <c r="K34" s="4">
+        <v>3</v>
+      </c>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4">
         <v>8.1929999999999996</v>
       </c>
-      <c r="K34" s="10" t="s">
+      <c r="N34" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="L34" s="3">
+      <c r="O34" s="3">
         <v>14</v>
       </c>
-      <c r="M34" s="4">
-        <v>4</v>
-      </c>
-      <c r="N34" s="57"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P34" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q34" s="57"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="64" t="s">
         <v>307</v>
       </c>
@@ -14436,14 +14870,19 @@
       </c>
       <c r="I35" s="64"/>
       <c r="J35" s="64">
+        <v>3</v>
+      </c>
+      <c r="K35" s="64"/>
+      <c r="L35" s="64"/>
+      <c r="M35" s="64">
         <v>20.204999999999998</v>
       </c>
-      <c r="K35" s="65"/>
-      <c r="L35" s="66"/>
-      <c r="M35" s="65"/>
-      <c r="N35" s="66"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N35" s="65"/>
+      <c r="O35" s="66"/>
+      <c r="P35" s="65"/>
+      <c r="Q35" s="66"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>307</v>
       </c>
@@ -14468,19 +14907,24 @@
         <v>6</v>
       </c>
       <c r="I36" s="4"/>
-      <c r="J36" s="4">
+      <c r="J36" s="4"/>
+      <c r="K36" s="4">
+        <v>3</v>
+      </c>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4">
         <v>20.204999999999998</v>
       </c>
-      <c r="K36" s="58" t="s">
+      <c r="N36" s="58" t="s">
         <v>321</v>
       </c>
-      <c r="L36" s="3">
-        <v>6</v>
-      </c>
-      <c r="M36" s="3"/>
-      <c r="N36" s="56"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36" s="3">
+        <v>6</v>
+      </c>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="56"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>307</v>
       </c>
@@ -14504,20 +14948,27 @@
         <f>Таблица6[[#This Row],[Годин 1 заїзд]]+Таблица6[[#This Row],[Годин 2 заїзд]]+-Таблица6[[#This Row],[Використано годин]]</f>
         <v>6</v>
       </c>
-      <c r="I37" s="4"/>
+      <c r="I37" s="4">
+        <v>3</v>
+      </c>
       <c r="J37" s="4">
+        <v>4</v>
+      </c>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4">
         <v>20.204999999999998</v>
       </c>
-      <c r="K37" s="58" t="s">
+      <c r="N37" s="58" t="s">
         <v>322</v>
       </c>
-      <c r="L37" s="56">
-        <v>6</v>
-      </c>
-      <c r="M37" s="3"/>
-      <c r="N37" s="56"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37" s="56">
+        <v>6</v>
+      </c>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="56"/>
+    </row>
+    <row r="38" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>307</v>
       </c>
@@ -14540,21 +14991,26 @@
         <v>6</v>
       </c>
       <c r="I38" s="4"/>
-      <c r="J38" s="4">
+      <c r="J38" s="4"/>
+      <c r="K38" s="4">
+        <v>3</v>
+      </c>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4">
         <v>20.204999999999998</v>
       </c>
-      <c r="K38" s="58" t="s">
+      <c r="N38" s="58" t="s">
         <v>220</v>
       </c>
-      <c r="L38" s="56">
-        <v>4</v>
-      </c>
-      <c r="M38" s="3"/>
-      <c r="N38" s="56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38" s="56">
+        <v>4</v>
+      </c>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>307</v>
       </c>
@@ -14577,21 +15033,26 @@
         <v>6</v>
       </c>
       <c r="I39" s="4"/>
-      <c r="J39" s="4">
+      <c r="J39" s="4"/>
+      <c r="K39" s="4">
+        <v>3</v>
+      </c>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4">
         <v>20.204999999999998</v>
       </c>
-      <c r="K39" s="58" t="s">
+      <c r="N39" s="58" t="s">
         <v>264</v>
       </c>
-      <c r="L39" s="56">
-        <v>4</v>
-      </c>
-      <c r="M39" s="3">
-        <v>2</v>
-      </c>
-      <c r="N39" s="56"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39" s="56">
+        <v>4</v>
+      </c>
+      <c r="P39" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q39" s="56"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="64" t="s">
         <v>307</v>
       </c>
@@ -14614,15 +15075,20 @@
         <v>6</v>
       </c>
       <c r="I40" s="64"/>
-      <c r="J40" s="64">
+      <c r="J40" s="64"/>
+      <c r="K40" s="64">
+        <v>2</v>
+      </c>
+      <c r="L40" s="64"/>
+      <c r="M40" s="64">
         <v>20.204999999999998</v>
       </c>
-      <c r="K40" s="65"/>
-      <c r="L40" s="67"/>
-      <c r="M40" s="65"/>
-      <c r="N40" s="67"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N40" s="65"/>
+      <c r="O40" s="67"/>
+      <c r="P40" s="65"/>
+      <c r="Q40" s="67"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>307</v>
       </c>
@@ -14646,20 +15112,27 @@
         <f>Таблица6[[#This Row],[Годин 1 заїзд]]+Таблица6[[#This Row],[Годин 2 заїзд]]+-Таблица6[[#This Row],[Використано годин]]</f>
         <v>6</v>
       </c>
-      <c r="I41" s="4"/>
+      <c r="I41" s="4">
+        <v>3</v>
+      </c>
       <c r="J41" s="4">
+        <v>4</v>
+      </c>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4">
         <v>20.204999999999998</v>
       </c>
-      <c r="K41" s="58" t="s">
+      <c r="N41" s="58" t="s">
         <v>323</v>
       </c>
-      <c r="L41" s="56">
-        <v>6</v>
-      </c>
-      <c r="M41" s="3"/>
-      <c r="N41" s="56"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41" s="56">
+        <v>6</v>
+      </c>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="56"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>307</v>
       </c>
@@ -14682,21 +15155,26 @@
         <v>8</v>
       </c>
       <c r="I42" s="4"/>
-      <c r="J42" s="4">
+      <c r="J42" s="4"/>
+      <c r="K42" s="4">
+        <v>3</v>
+      </c>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4">
         <v>20.204999999999998</v>
       </c>
-      <c r="K42" s="58" t="s">
+      <c r="N42" s="58" t="s">
         <v>207</v>
       </c>
-      <c r="L42" s="56">
-        <v>6</v>
-      </c>
-      <c r="M42" s="3">
-        <v>2</v>
-      </c>
-      <c r="N42" s="56"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42" s="56">
+        <v>6</v>
+      </c>
+      <c r="P42" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q42" s="56"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="64" t="s">
         <v>307</v>
       </c>
@@ -14722,14 +15200,19 @@
       </c>
       <c r="I43" s="64"/>
       <c r="J43" s="64">
+        <v>4</v>
+      </c>
+      <c r="K43" s="64"/>
+      <c r="L43" s="64"/>
+      <c r="M43" s="64">
         <v>20.204999999999998</v>
       </c>
-      <c r="K43" s="65"/>
-      <c r="L43" s="67"/>
-      <c r="M43" s="65"/>
-      <c r="N43" s="67"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N43" s="65"/>
+      <c r="O43" s="67"/>
+      <c r="P43" s="65"/>
+      <c r="Q43" s="67"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="64" t="s">
         <v>307</v>
       </c>
@@ -14754,15 +15237,20 @@
         <v>4</v>
       </c>
       <c r="I44" s="64"/>
-      <c r="J44" s="64">
+      <c r="J44" s="64"/>
+      <c r="K44" s="64">
+        <v>4</v>
+      </c>
+      <c r="L44" s="64"/>
+      <c r="M44" s="64">
         <v>20.204999999999998</v>
       </c>
-      <c r="K44" s="65"/>
-      <c r="L44" s="67"/>
-      <c r="M44" s="65"/>
-      <c r="N44" s="67"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N44" s="65"/>
+      <c r="O44" s="67"/>
+      <c r="P44" s="65"/>
+      <c r="Q44" s="67"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="64" t="s">
         <v>307</v>
       </c>
@@ -14787,15 +15275,20 @@
         <v>6</v>
       </c>
       <c r="I45" s="64"/>
-      <c r="J45" s="64">
+      <c r="J45" s="64"/>
+      <c r="K45" s="64">
+        <v>4</v>
+      </c>
+      <c r="L45" s="64"/>
+      <c r="M45" s="64">
         <v>20.204999999999998</v>
       </c>
-      <c r="K45" s="65"/>
-      <c r="L45" s="67"/>
-      <c r="M45" s="65"/>
-      <c r="N45" s="67"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N45" s="65"/>
+      <c r="O45" s="67"/>
+      <c r="P45" s="65"/>
+      <c r="Q45" s="67"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>307</v>
       </c>
@@ -14819,20 +15312,27 @@
         <f>Таблица6[[#This Row],[Годин 1 заїзд]]+Таблица6[[#This Row],[Годин 2 заїзд]]+-Таблица6[[#This Row],[Використано годин]]</f>
         <v>6</v>
       </c>
-      <c r="I46" s="4"/>
+      <c r="I46" s="4">
+        <v>3</v>
+      </c>
       <c r="J46" s="4">
+        <v>4</v>
+      </c>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4">
         <v>20.204999999999998</v>
       </c>
-      <c r="K46" s="58" t="s">
+      <c r="N46" s="58" t="s">
         <v>324</v>
       </c>
-      <c r="L46" s="56">
-        <v>6</v>
-      </c>
-      <c r="M46" s="3"/>
-      <c r="N46" s="56"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46" s="56">
+        <v>6</v>
+      </c>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="56"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>307</v>
       </c>
@@ -14858,18 +15358,23 @@
       </c>
       <c r="I47" s="4"/>
       <c r="J47" s="4">
+        <v>3</v>
+      </c>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4">
         <v>20.204999999999998</v>
       </c>
-      <c r="K47" s="58" t="s">
+      <c r="N47" s="58" t="s">
         <v>325</v>
       </c>
-      <c r="L47" s="56">
-        <v>6</v>
-      </c>
-      <c r="M47" s="3"/>
-      <c r="N47" s="56"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47" s="56">
+        <v>6</v>
+      </c>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="56"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>307</v>
       </c>
@@ -14893,20 +15398,25 @@
       </c>
       <c r="I48" s="4"/>
       <c r="J48" s="4">
+        <v>3</v>
+      </c>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4">
         <v>20.204999999999998</v>
       </c>
-      <c r="K48" s="58" t="s">
+      <c r="N48" s="58" t="s">
         <v>321</v>
       </c>
-      <c r="L48" s="56">
-        <v>6</v>
-      </c>
-      <c r="M48" s="3"/>
-      <c r="N48" s="56"/>
+      <c r="O48" s="56">
+        <v>6</v>
+      </c>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>

</xml_diff>